<commit_message>
Agregando Santa Rosa de Viterbo
</commit_message>
<xml_diff>
--- a/Bases_de_Rama_Judicial-Cálculo_DEA.xlsx
+++ b/Bases_de_Rama_Judicial-Cálculo_DEA.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1800" windowWidth="24000" windowHeight="9216" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="2400" windowWidth="24000" windowHeight="9216"/>
   </bookViews>
   <sheets>
     <sheet name="circuito" sheetId="5" r:id="rId1"/>
@@ -34,7 +34,7 @@
     <author>Manuel Felipe Diaz Rangel</author>
   </authors>
   <commentList>
-    <comment ref="E38" authorId="0" shapeId="0">
+    <comment ref="E31" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -96,8 +96,42 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Manuel Felipe Diaz Rangel</author>
+  </authors>
+  <commentList>
+    <comment ref="E38" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Manuel Felipe Diaz Rangel:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+No se encontró número de jueces en la base de Despacho</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="86">
   <si>
     <t>Competencia</t>
   </si>
@@ -334,6 +368,27 @@
   </si>
   <si>
     <t>Cauca</t>
+  </si>
+  <si>
+    <t>Ante la falta de información con respecto al número de jueces de Santarosa de Viterbo, se procede a promediar un número de jueces teniendo en cuenta circuitos con ingresos y egresos similares</t>
+  </si>
+  <si>
+    <t>ingresos</t>
+  </si>
+  <si>
+    <t>egresos</t>
+  </si>
+  <si>
+    <t>Santarosa</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>jueces</t>
+  </si>
+  <si>
+    <t>El número de jueces de Santa Rosa de Viterbo sería un promedio de 7</t>
   </si>
 </sst>
 </file>
@@ -434,7 +489,7 @@
     <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -468,6 +523,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -750,10 +811,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1272,215 +1335,234 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="8" t="s">
-        <v>25</v>
+      <c r="A31" s="13" t="s">
+        <v>10</v>
       </c>
       <c r="B31" s="5">
-        <v>267</v>
+        <v>323</v>
       </c>
       <c r="C31" s="5">
-        <v>181</v>
+        <v>129</v>
       </c>
       <c r="D31" s="5">
-        <v>774</v>
-      </c>
-      <c r="E31" s="8">
-        <v>8</v>
+        <v>210</v>
+      </c>
+      <c r="E31" s="4">
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="B32" s="5">
-        <v>243</v>
+        <v>267</v>
       </c>
       <c r="C32" s="5">
-        <v>153</v>
+        <v>181</v>
       </c>
       <c r="D32" s="5">
-        <v>549</v>
+        <v>774</v>
       </c>
       <c r="E32" s="8">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="B33" s="5">
-        <v>180</v>
+        <v>243</v>
       </c>
       <c r="C33" s="5">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="D33" s="5">
-        <v>327</v>
+        <v>549</v>
       </c>
       <c r="E33" s="8">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B34" s="5">
-        <v>102</v>
+        <v>180</v>
       </c>
       <c r="C34" s="5">
-        <v>38</v>
+        <v>159</v>
       </c>
       <c r="D34" s="5">
-        <v>219</v>
+        <v>327</v>
       </c>
       <c r="E34" s="8">
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="B35" s="5">
-        <v>631</v>
+        <v>102</v>
       </c>
       <c r="C35" s="5">
-        <v>272</v>
+        <v>38</v>
       </c>
       <c r="D35" s="5">
-        <v>1235</v>
+        <v>219</v>
       </c>
       <c r="E35" s="8">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="B36" s="5">
-        <v>427</v>
+        <v>631</v>
       </c>
       <c r="C36" s="5">
-        <v>378</v>
+        <v>272</v>
       </c>
       <c r="D36" s="5">
-        <v>894</v>
+        <v>1235</v>
       </c>
       <c r="E36" s="8">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="B37" s="5">
-        <v>124</v>
+        <v>427</v>
       </c>
       <c r="C37" s="5">
-        <v>22</v>
+        <v>378</v>
       </c>
       <c r="D37" s="5">
-        <v>319</v>
+        <v>894</v>
       </c>
       <c r="E37" s="8">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" s="5">
+        <v>124</v>
+      </c>
+      <c r="C38" s="5">
         <v>22</v>
       </c>
-      <c r="B38" s="5">
+      <c r="D38" s="5">
+        <v>319</v>
+      </c>
+      <c r="E38" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B39" s="5">
         <v>28</v>
       </c>
-      <c r="C38" s="5">
+      <c r="C39" s="5">
         <v>23</v>
       </c>
-      <c r="D38" s="5">
+      <c r="D39" s="5">
         <v>32</v>
       </c>
-      <c r="E38" s="8">
+      <c r="E39" s="8">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:E5"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.8984375" customWidth="1"/>
+    <col min="11" max="11" width="11.8984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5" s="14">
         <v>2016</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>54</v>
       </c>
@@ -1497,7 +1579,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -1513,8 +1595,14 @@
       <c r="E8" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H8" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
@@ -1530,8 +1618,12 @@
       <c r="E9" s="1">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>33</v>
       </c>
@@ -1547,8 +1639,12 @@
       <c r="E10" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -1564,8 +1660,12 @@
       <c r="E11" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
@@ -1582,7 +1682,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>34</v>
       </c>
@@ -1598,8 +1698,20 @@
       <c r="E13" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H13" t="s">
+        <v>82</v>
+      </c>
+      <c r="I13">
+        <v>323</v>
+      </c>
+      <c r="J13">
+        <v>129</v>
+      </c>
+      <c r="K13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>38</v>
       </c>
@@ -1616,7 +1728,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>39</v>
       </c>
@@ -1632,8 +1744,17 @@
       <c r="E15" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I15" t="s">
+        <v>80</v>
+      </c>
+      <c r="J15" t="s">
+        <v>81</v>
+      </c>
+      <c r="K15" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>40</v>
       </c>
@@ -1650,7 +1771,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>9</v>
       </c>
@@ -1666,8 +1787,20 @@
       <c r="E17" s="1">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
+        <v>39</v>
+      </c>
+      <c r="I17">
+        <v>352</v>
+      </c>
+      <c r="J17">
+        <v>122</v>
+      </c>
+      <c r="K17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>29</v>
       </c>
@@ -1683,8 +1816,20 @@
       <c r="E18" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>29</v>
+      </c>
+      <c r="I18">
+        <v>317</v>
+      </c>
+      <c r="J18">
+        <v>102</v>
+      </c>
+      <c r="K18">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>41</v>
       </c>
@@ -1700,8 +1845,20 @@
       <c r="E19" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
+        <v>18</v>
+      </c>
+      <c r="I19">
+        <v>309</v>
+      </c>
+      <c r="J19">
+        <v>121</v>
+      </c>
+      <c r="K19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>13</v>
       </c>
@@ -1718,7 +1875,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -1734,8 +1891,12 @@
       <c r="E21" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="K21">
+        <f>AVERAGE(K17,K18,K19)</f>
+        <v>6.666666666666667</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>37</v>
       </c>
@@ -1752,7 +1913,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -1769,7 +1930,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>12</v>
       </c>
@@ -1785,8 +1946,11 @@
       <c r="E24" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H24" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>4</v>
       </c>
@@ -1803,7 +1967,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>27</v>
       </c>
@@ -1820,7 +1984,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>18</v>
       </c>
@@ -1837,7 +2001,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>23</v>
       </c>
@@ -1854,7 +2018,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>30</v>
       </c>
@@ -1871,7 +2035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
@@ -1888,7 +2052,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>32</v>
       </c>
@@ -1905,7 +2069,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>15</v>
       </c>
@@ -2162,7 +2326,8 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="H8:K11"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
@@ -2178,7 +2343,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A19" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2190,56 +2355,56 @@
       <c r="A1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5" s="14">
         <v>2016</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -3329,56 +3494,56 @@
       <c r="A1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5" s="14">
         <v>2016</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">

</xml_diff>

<commit_message>
Actualizando bases de datos con nueva variable: Carga
</commit_message>
<xml_diff>
--- a/Bases_de_Rama_Judicial-Cálculo_DEA.xlsx
+++ b/Bases_de_Rama_Judicial-Cálculo_DEA.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2400" windowWidth="24000" windowHeight="9216"/>
+    <workbookView xWindow="0" yWindow="3000" windowWidth="24000" windowHeight="9216" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="circuito" sheetId="5" r:id="rId1"/>
@@ -131,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="88">
   <si>
     <t>Competencia</t>
   </si>
@@ -389,6 +389,12 @@
   </si>
   <si>
     <t>El número de jueces de Santa Rosa de Viterbo sería un promedio de 7</t>
+  </si>
+  <si>
+    <t>Carga</t>
+  </si>
+  <si>
+    <t>Esto no tiene interpretación, sirve solo para comparar contra los tribunales</t>
   </si>
 </sst>
 </file>
@@ -489,7 +495,7 @@
     <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -524,12 +530,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Millares [0] 2" xfId="1"/>
@@ -812,10 +819,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -824,7 +831,7 @@
     <col min="2" max="16384" width="11.19921875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>54</v>
       </c>
@@ -840,8 +847,11 @@
       <c r="E1" s="3" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>6</v>
       </c>
@@ -857,8 +867,12 @@
       <c r="E2" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="16">
+        <f>SUM(B2,D2)</f>
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>31</v>
       </c>
@@ -874,8 +888,12 @@
       <c r="E3" s="8">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="16">
+        <f t="shared" ref="F3:F39" si="0">SUM(B3,D3)</f>
+        <v>670</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>33</v>
       </c>
@@ -891,8 +909,12 @@
       <c r="E4" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="16">
+        <f t="shared" si="0"/>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>8</v>
       </c>
@@ -908,8 +930,12 @@
       <c r="E5" s="8">
         <v>15</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="16">
+        <f t="shared" si="0"/>
+        <v>1835</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>19</v>
       </c>
@@ -925,8 +951,12 @@
       <c r="E6" s="8">
         <v>65</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="16">
+        <f t="shared" si="0"/>
+        <v>10558</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>34</v>
       </c>
@@ -942,8 +972,12 @@
       <c r="E7" s="8">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="16">
+        <f t="shared" si="0"/>
+        <v>987</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>38</v>
       </c>
@@ -959,8 +993,12 @@
       <c r="E8" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="16">
+        <f t="shared" si="0"/>
+        <v>328</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>39</v>
       </c>
@@ -976,8 +1014,12 @@
       <c r="E9" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="16">
+        <f t="shared" si="0"/>
+        <v>944</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>40</v>
       </c>
@@ -993,8 +1035,12 @@
       <c r="E10" s="8">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="16">
+        <f t="shared" si="0"/>
+        <v>3440</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>9</v>
       </c>
@@ -1010,8 +1056,12 @@
       <c r="E11" s="8">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" s="16">
+        <f t="shared" si="0"/>
+        <v>2253</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>29</v>
       </c>
@@ -1027,8 +1077,12 @@
       <c r="E12" s="8">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="16">
+        <f t="shared" si="0"/>
+        <v>1372</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>41</v>
       </c>
@@ -1044,8 +1098,12 @@
       <c r="E13" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" s="16">
+        <f t="shared" si="0"/>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>13</v>
       </c>
@@ -1061,8 +1119,12 @@
       <c r="E14" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" s="16">
+        <f t="shared" si="0"/>
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>20</v>
       </c>
@@ -1078,8 +1140,12 @@
       <c r="E15" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15" s="16">
+        <f t="shared" si="0"/>
+        <v>187</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>37</v>
       </c>
@@ -1095,8 +1161,12 @@
       <c r="E16" s="8">
         <v>12</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" s="16">
+        <f t="shared" si="0"/>
+        <v>1785</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>21</v>
       </c>
@@ -1112,8 +1182,12 @@
       <c r="E17" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" s="16">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>12</v>
       </c>
@@ -1129,8 +1203,12 @@
       <c r="E18" s="8">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" s="16">
+        <f t="shared" si="0"/>
+        <v>886</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>4</v>
       </c>
@@ -1146,8 +1224,12 @@
       <c r="E19" s="8">
         <v>36</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" s="16">
+        <f t="shared" si="0"/>
+        <v>4656</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>27</v>
       </c>
@@ -1163,8 +1245,12 @@
       <c r="E20" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" s="16">
+        <f t="shared" si="0"/>
+        <v>900</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>18</v>
       </c>
@@ -1180,8 +1266,12 @@
       <c r="E21" s="8">
         <v>7</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" s="16">
+        <f t="shared" si="0"/>
+        <v>981</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>23</v>
       </c>
@@ -1197,8 +1287,12 @@
       <c r="E22" s="8">
         <v>9</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" s="16">
+        <f t="shared" si="0"/>
+        <v>1485</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>30</v>
       </c>
@@ -1214,8 +1308,12 @@
       <c r="E23" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23" s="16">
+        <f t="shared" si="0"/>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>28</v>
       </c>
@@ -1231,8 +1329,12 @@
       <c r="E24" s="8">
         <v>9</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" s="16">
+        <f t="shared" si="0"/>
+        <v>1541</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>32</v>
       </c>
@@ -1248,8 +1350,12 @@
       <c r="E25" s="8">
         <v>7</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" s="16">
+        <f t="shared" si="0"/>
+        <v>797</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>15</v>
       </c>
@@ -1265,8 +1371,12 @@
       <c r="E26" s="8">
         <v>10</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26" s="16">
+        <f t="shared" si="0"/>
+        <v>3071</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>17</v>
       </c>
@@ -1282,8 +1392,12 @@
       <c r="E27" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27" s="16">
+        <f t="shared" si="0"/>
+        <v>964</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>24</v>
       </c>
@@ -1299,8 +1413,12 @@
       <c r="E28" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28" s="16">
+        <f t="shared" si="0"/>
+        <v>591</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>7</v>
       </c>
@@ -1316,8 +1434,12 @@
       <c r="E29" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29" s="16">
+        <f t="shared" si="0"/>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>35</v>
       </c>
@@ -1333,8 +1455,12 @@
       <c r="E30" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30" s="16">
+        <f t="shared" si="0"/>
+        <v>301</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="13" t="s">
         <v>10</v>
       </c>
@@ -1350,8 +1476,12 @@
       <c r="E31" s="4">
         <v>7</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31" s="16">
+        <f t="shared" si="0"/>
+        <v>533</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>25</v>
       </c>
@@ -1367,8 +1497,12 @@
       <c r="E32" s="8">
         <v>8</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32" s="16">
+        <f t="shared" si="0"/>
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>36</v>
       </c>
@@ -1384,8 +1518,12 @@
       <c r="E33" s="8">
         <v>9</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33" s="16">
+        <f t="shared" si="0"/>
+        <v>792</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>11</v>
       </c>
@@ -1401,8 +1539,12 @@
       <c r="E34" s="8">
         <v>15</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34" s="16">
+        <f t="shared" si="0"/>
+        <v>507</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
         <v>5</v>
       </c>
@@ -1418,8 +1560,12 @@
       <c r="E35" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35" s="16">
+        <f t="shared" si="0"/>
+        <v>321</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>16</v>
       </c>
@@ -1435,8 +1581,12 @@
       <c r="E36" s="8">
         <v>8</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36" s="16">
+        <f t="shared" si="0"/>
+        <v>1866</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
         <v>26</v>
       </c>
@@ -1452,8 +1602,12 @@
       <c r="E37" s="8">
         <v>9</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F37" s="16">
+        <f t="shared" si="0"/>
+        <v>1321</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
         <v>14</v>
       </c>
@@ -1469,8 +1623,12 @@
       <c r="E38" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F38" s="16">
+        <f t="shared" si="0"/>
+        <v>443</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
         <v>22</v>
       </c>
@@ -1485,6 +1643,10 @@
       </c>
       <c r="E39" s="8">
         <v>3</v>
+      </c>
+      <c r="F39" s="16">
+        <f t="shared" si="0"/>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1497,8 +1659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1511,56 +1673,56 @@
       <c r="A1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="15">
         <v>2016</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -1595,12 +1757,12 @@
       <c r="E8" s="1">
         <v>2</v>
       </c>
-      <c r="H8" s="15" t="s">
+      <c r="H8" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -1618,10 +1780,10 @@
       <c r="E9" s="1">
         <v>6</v>
       </c>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -1639,10 +1801,10 @@
       <c r="E10" s="1">
         <v>2</v>
       </c>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -1660,10 +1822,10 @@
       <c r="E11" s="1">
         <v>15</v>
       </c>
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -2341,9 +2503,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2351,62 +2515,62 @@
     <col min="2" max="16384" width="11.19921875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="15">
         <v>2016</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>53</v>
       </c>
@@ -2423,7 +2587,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>55</v>
       </c>
@@ -2442,7 +2606,7 @@
       <c r="G8" s="10"/>
       <c r="H8" s="12"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>6</v>
       </c>
@@ -2461,7 +2625,7 @@
       <c r="G9" s="10"/>
       <c r="H9" s="12"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>56</v>
       </c>
@@ -2477,10 +2641,13 @@
       <c r="E10" s="8">
         <v>15</v>
       </c>
-      <c r="G10" s="10"/>
-      <c r="H10" s="12"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G10" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>57</v>
       </c>
@@ -2496,10 +2663,11 @@
       <c r="E11" s="8">
         <v>15</v>
       </c>
-      <c r="G11" s="10"/>
-      <c r="H11" s="12"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>58</v>
       </c>
@@ -2515,10 +2683,11 @@
       <c r="E12" s="8">
         <v>19</v>
       </c>
-      <c r="G12" s="10"/>
-      <c r="H12" s="12"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>59</v>
       </c>
@@ -2534,10 +2703,11 @@
       <c r="E13" s="8">
         <v>8</v>
       </c>
-      <c r="G13" s="10"/>
-      <c r="H13" s="12"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>60</v>
       </c>
@@ -2556,7 +2726,7 @@
       <c r="G14" s="10"/>
       <c r="H14" s="12"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>61</v>
       </c>
@@ -2575,7 +2745,7 @@
       <c r="G15" s="10"/>
       <c r="H15" s="12"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>78</v>
       </c>
@@ -2938,7 +3108,8 @@
       <c r="H34" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="G10:I13"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
@@ -2954,7 +3125,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="H20" sqref="H20:H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -2979,6 +3150,9 @@
       <c r="E1" s="3" t="s">
         <v>51</v>
       </c>
+      <c r="F1" s="3" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
@@ -2996,6 +3170,10 @@
       <c r="E2" s="7">
         <v>38</v>
       </c>
+      <c r="F2" s="16">
+        <f>SUM(B2,D2)</f>
+        <v>4977</v>
+      </c>
       <c r="G2" s="10"/>
       <c r="H2" s="11"/>
     </row>
@@ -3015,6 +3193,10 @@
       <c r="E3" s="7">
         <v>2</v>
       </c>
+      <c r="F3" s="16">
+        <f t="shared" ref="F3:F27" si="0">SUM(B3,D3)</f>
+        <v>1076</v>
+      </c>
       <c r="G3" s="10"/>
       <c r="H3" s="11"/>
     </row>
@@ -3034,6 +3216,10 @@
       <c r="E4" s="7">
         <v>15</v>
       </c>
+      <c r="F4" s="16">
+        <f t="shared" si="0"/>
+        <v>1835</v>
+      </c>
       <c r="G4" s="10"/>
       <c r="H4" s="11"/>
     </row>
@@ -3053,6 +3239,10 @@
       <c r="E5" s="7">
         <v>15</v>
       </c>
+      <c r="F5" s="16">
+        <f t="shared" si="0"/>
+        <v>2253</v>
+      </c>
       <c r="G5" s="10"/>
       <c r="H5" s="11"/>
     </row>
@@ -3072,6 +3262,10 @@
       <c r="E6" s="7">
         <v>19</v>
       </c>
+      <c r="F6" s="16">
+        <f t="shared" si="0"/>
+        <v>1040</v>
+      </c>
       <c r="G6" s="10"/>
       <c r="H6" s="11"/>
     </row>
@@ -3091,6 +3285,10 @@
       <c r="E7" s="7">
         <v>8</v>
       </c>
+      <c r="F7" s="16">
+        <f t="shared" si="0"/>
+        <v>886</v>
+      </c>
       <c r="G7" s="10"/>
       <c r="H7" s="11"/>
     </row>
@@ -3110,6 +3308,10 @@
       <c r="E8" s="7">
         <v>4</v>
       </c>
+      <c r="F8" s="16">
+        <f t="shared" si="0"/>
+        <v>1751</v>
+      </c>
       <c r="G8" s="10"/>
       <c r="H8" s="11"/>
     </row>
@@ -3129,6 +3331,10 @@
       <c r="E9" s="7">
         <v>2</v>
       </c>
+      <c r="F9" s="16">
+        <f t="shared" si="0"/>
+        <v>443</v>
+      </c>
       <c r="G9" s="10"/>
       <c r="H9" s="11"/>
     </row>
@@ -3148,6 +3354,10 @@
       <c r="E10" s="7">
         <v>10</v>
       </c>
+      <c r="F10" s="16">
+        <f t="shared" si="0"/>
+        <v>3071</v>
+      </c>
       <c r="G10" s="10"/>
       <c r="H10" s="11"/>
     </row>
@@ -3167,6 +3377,10 @@
       <c r="E11" s="7">
         <v>8</v>
       </c>
+      <c r="F11" s="16">
+        <f t="shared" si="0"/>
+        <v>1866</v>
+      </c>
       <c r="G11" s="10"/>
       <c r="H11" s="11"/>
     </row>
@@ -3186,6 +3400,10 @@
       <c r="E12" s="7">
         <v>4</v>
       </c>
+      <c r="F12" s="16">
+        <f t="shared" si="0"/>
+        <v>964</v>
+      </c>
       <c r="G12" s="10"/>
       <c r="H12" s="11"/>
     </row>
@@ -3205,6 +3423,10 @@
       <c r="E13" s="7">
         <v>7</v>
       </c>
+      <c r="F13" s="16">
+        <f t="shared" si="0"/>
+        <v>981</v>
+      </c>
       <c r="G13" s="10"/>
       <c r="H13" s="11"/>
     </row>
@@ -3224,6 +3446,10 @@
       <c r="E14" s="7">
         <v>75</v>
       </c>
+      <c r="F14" s="16">
+        <f t="shared" si="0"/>
+        <v>10948</v>
+      </c>
       <c r="G14" s="10"/>
       <c r="H14" s="11"/>
     </row>
@@ -3243,6 +3469,10 @@
       <c r="E15" s="7">
         <v>3</v>
       </c>
+      <c r="F15" s="16">
+        <f t="shared" si="0"/>
+        <v>591</v>
+      </c>
       <c r="G15" s="10"/>
       <c r="H15" s="11"/>
     </row>
@@ -3262,6 +3492,10 @@
       <c r="E16" s="7">
         <v>9</v>
       </c>
+      <c r="F16" s="16">
+        <f t="shared" si="0"/>
+        <v>1485</v>
+      </c>
       <c r="G16" s="10"/>
       <c r="H16" s="11"/>
     </row>
@@ -3281,6 +3515,10 @@
       <c r="E17" s="7">
         <v>8</v>
       </c>
+      <c r="F17" s="16">
+        <f t="shared" si="0"/>
+        <v>1041</v>
+      </c>
       <c r="G17" s="10"/>
       <c r="H17" s="11"/>
     </row>
@@ -3300,6 +3538,10 @@
       <c r="E18" s="7">
         <v>9</v>
       </c>
+      <c r="F18" s="16">
+        <f t="shared" si="0"/>
+        <v>1321</v>
+      </c>
       <c r="G18" s="10"/>
       <c r="H18" s="11"/>
     </row>
@@ -3319,6 +3561,10 @@
       <c r="E19" s="7">
         <v>11</v>
       </c>
+      <c r="F19" s="16">
+        <f t="shared" si="0"/>
+        <v>2441</v>
+      </c>
       <c r="G19" s="10"/>
       <c r="H19" s="11"/>
     </row>
@@ -3338,6 +3584,10 @@
       <c r="E20" s="7">
         <v>11</v>
       </c>
+      <c r="F20" s="16">
+        <f t="shared" si="0"/>
+        <v>1477</v>
+      </c>
       <c r="G20" s="10"/>
       <c r="H20" s="11"/>
     </row>
@@ -3357,6 +3607,10 @@
       <c r="E21" s="7">
         <v>6</v>
       </c>
+      <c r="F21" s="16">
+        <f t="shared" si="0"/>
+        <v>670</v>
+      </c>
       <c r="G21" s="10"/>
       <c r="H21" s="11"/>
     </row>
@@ -3376,6 +3630,10 @@
       <c r="E22" s="7">
         <v>7</v>
       </c>
+      <c r="F22" s="16">
+        <f t="shared" si="0"/>
+        <v>797</v>
+      </c>
       <c r="G22" s="10"/>
       <c r="H22" s="11"/>
     </row>
@@ -3395,6 +3653,10 @@
       <c r="E23" s="7">
         <v>1</v>
       </c>
+      <c r="F23" s="16">
+        <f t="shared" si="0"/>
+        <v>135</v>
+      </c>
       <c r="G23" s="10"/>
       <c r="H23" s="11"/>
     </row>
@@ -3414,6 +3676,10 @@
       <c r="E24" s="7">
         <v>20</v>
       </c>
+      <c r="F24" s="16">
+        <f t="shared" si="0"/>
+        <v>1458</v>
+      </c>
       <c r="G24" s="10"/>
       <c r="H24" s="11"/>
     </row>
@@ -3433,6 +3699,10 @@
       <c r="E25" s="7">
         <v>9</v>
       </c>
+      <c r="F25" s="16">
+        <f t="shared" si="0"/>
+        <v>792</v>
+      </c>
       <c r="G25" s="10"/>
       <c r="H25" s="11"/>
     </row>
@@ -3452,6 +3722,10 @@
       <c r="E26" s="7">
         <v>12</v>
       </c>
+      <c r="F26" s="16">
+        <f t="shared" si="0"/>
+        <v>1785</v>
+      </c>
       <c r="G26" s="10"/>
       <c r="H26" s="11"/>
     </row>
@@ -3470,6 +3744,10 @@
       </c>
       <c r="E27" s="7">
         <v>29</v>
+      </c>
+      <c r="F27" s="16">
+        <f t="shared" si="0"/>
+        <v>4712</v>
       </c>
       <c r="G27" s="10"/>
       <c r="H27" s="11"/>
@@ -3494,56 +3772,56 @@
       <c r="A1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="15">
         <v>2016</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -4178,7 +4456,7 @@
   <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -4203,6 +4481,9 @@
       <c r="E1" s="3" t="s">
         <v>51</v>
       </c>
+      <c r="F1" s="3" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
@@ -4220,6 +4501,10 @@
       <c r="E2" s="8">
         <v>15</v>
       </c>
+      <c r="F2" s="16">
+        <f>SUM(B2,D2)</f>
+        <v>2465</v>
+      </c>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
     </row>
@@ -4239,6 +4524,10 @@
       <c r="E3" s="8">
         <v>3</v>
       </c>
+      <c r="F3" s="16">
+        <f t="shared" ref="F3:F27" si="0">SUM(B3,D3)</f>
+        <v>212</v>
+      </c>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
     </row>
@@ -4258,6 +4547,10 @@
       <c r="E4" s="8">
         <v>9</v>
       </c>
+      <c r="F4" s="16">
+        <f t="shared" si="0"/>
+        <v>793</v>
+      </c>
       <c r="G4" s="12"/>
       <c r="H4" s="12"/>
     </row>
@@ -4277,6 +4570,10 @@
       <c r="E5" s="8">
         <v>6</v>
       </c>
+      <c r="F5" s="16">
+        <f t="shared" si="0"/>
+        <v>1019</v>
+      </c>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
     </row>
@@ -4296,6 +4593,10 @@
       <c r="E6" s="8">
         <v>6</v>
       </c>
+      <c r="F6" s="16">
+        <f t="shared" si="0"/>
+        <v>653</v>
+      </c>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
     </row>
@@ -4315,6 +4616,10 @@
       <c r="E7" s="8">
         <v>6</v>
       </c>
+      <c r="F7" s="16">
+        <f t="shared" si="0"/>
+        <v>415</v>
+      </c>
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
     </row>
@@ -4334,6 +4639,10 @@
       <c r="E8" s="8">
         <v>4</v>
       </c>
+      <c r="F8" s="16">
+        <f t="shared" si="0"/>
+        <v>1012</v>
+      </c>
       <c r="G8" s="12"/>
       <c r="H8" s="12"/>
     </row>
@@ -4353,6 +4662,10 @@
       <c r="E9" s="8">
         <v>3</v>
       </c>
+      <c r="F9" s="16">
+        <f t="shared" si="0"/>
+        <v>224</v>
+      </c>
       <c r="G9" s="12"/>
       <c r="H9" s="12"/>
     </row>
@@ -4372,6 +4685,10 @@
       <c r="E10" s="8">
         <v>5</v>
       </c>
+      <c r="F10" s="16">
+        <f t="shared" si="0"/>
+        <v>1071</v>
+      </c>
       <c r="G10" s="12"/>
       <c r="H10" s="12"/>
     </row>
@@ -4391,6 +4708,10 @@
       <c r="E11" s="8">
         <v>4</v>
       </c>
+      <c r="F11" s="16">
+        <f t="shared" si="0"/>
+        <v>638</v>
+      </c>
       <c r="G11" s="12"/>
       <c r="H11" s="12"/>
     </row>
@@ -4410,6 +4731,10 @@
       <c r="E12" s="8">
         <v>3</v>
       </c>
+      <c r="F12" s="16">
+        <f t="shared" si="0"/>
+        <v>348</v>
+      </c>
       <c r="G12" s="12"/>
       <c r="H12" s="12"/>
     </row>
@@ -4429,6 +4754,10 @@
       <c r="E13" s="8">
         <v>4</v>
       </c>
+      <c r="F13" s="16">
+        <f t="shared" si="0"/>
+        <v>471</v>
+      </c>
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
     </row>
@@ -4448,6 +4777,10 @@
       <c r="E14" s="8">
         <v>9</v>
       </c>
+      <c r="F14" s="16">
+        <f t="shared" si="0"/>
+        <v>3729</v>
+      </c>
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
     </row>
@@ -4467,6 +4800,10 @@
       <c r="E15" s="8">
         <v>3</v>
       </c>
+      <c r="F15" s="16">
+        <f t="shared" si="0"/>
+        <v>180</v>
+      </c>
       <c r="G15" s="12"/>
       <c r="H15" s="12"/>
     </row>
@@ -4486,6 +4823,10 @@
       <c r="E16" s="8">
         <v>6</v>
       </c>
+      <c r="F16" s="16">
+        <f t="shared" si="0"/>
+        <v>486</v>
+      </c>
       <c r="G16" s="12"/>
       <c r="H16" s="12"/>
     </row>
@@ -4505,6 +4846,10 @@
       <c r="E17" s="8">
         <v>4</v>
       </c>
+      <c r="F17" s="16">
+        <f t="shared" si="0"/>
+        <v>506</v>
+      </c>
       <c r="G17" s="12"/>
       <c r="H17" s="12"/>
     </row>
@@ -4524,6 +4869,10 @@
       <c r="E18" s="8">
         <v>5</v>
       </c>
+      <c r="F18" s="16">
+        <f t="shared" si="0"/>
+        <v>1539</v>
+      </c>
       <c r="G18" s="12"/>
       <c r="H18" s="12"/>
     </row>
@@ -4543,6 +4892,10 @@
       <c r="E19" s="8">
         <v>6</v>
       </c>
+      <c r="F19" s="16">
+        <f t="shared" si="0"/>
+        <v>1263</v>
+      </c>
       <c r="G19" s="12"/>
       <c r="H19" s="12"/>
     </row>
@@ -4562,6 +4915,10 @@
       <c r="E20" s="8">
         <v>5</v>
       </c>
+      <c r="F20" s="16">
+        <f t="shared" si="0"/>
+        <v>675</v>
+      </c>
       <c r="G20" s="12"/>
       <c r="H20" s="12"/>
     </row>
@@ -4581,6 +4938,10 @@
       <c r="E21" s="8">
         <v>5</v>
       </c>
+      <c r="F21" s="16">
+        <f t="shared" si="0"/>
+        <v>521</v>
+      </c>
       <c r="G21" s="12"/>
       <c r="H21" s="12"/>
     </row>
@@ -4600,6 +4961,10 @@
       <c r="E22" s="8">
         <v>4</v>
       </c>
+      <c r="F22" s="16">
+        <f t="shared" si="0"/>
+        <v>559</v>
+      </c>
       <c r="G22" s="12"/>
       <c r="H22" s="12"/>
     </row>
@@ -4619,6 +4984,10 @@
       <c r="E23" s="8">
         <v>3</v>
       </c>
+      <c r="F23" s="16">
+        <f t="shared" si="0"/>
+        <v>101</v>
+      </c>
       <c r="G23" s="12"/>
       <c r="H23" s="12"/>
     </row>
@@ -4638,6 +5007,10 @@
       <c r="E24" s="8">
         <v>6</v>
       </c>
+      <c r="F24" s="16">
+        <f t="shared" si="0"/>
+        <v>974</v>
+      </c>
       <c r="G24" s="12"/>
       <c r="H24" s="12"/>
     </row>
@@ -4657,6 +5030,10 @@
       <c r="E25" s="8">
         <v>4</v>
       </c>
+      <c r="F25" s="16">
+        <f t="shared" si="0"/>
+        <v>438</v>
+      </c>
       <c r="G25" s="12"/>
       <c r="H25" s="12"/>
     </row>
@@ -4676,6 +5053,10 @@
       <c r="E26" s="8">
         <v>6</v>
       </c>
+      <c r="F26" s="16">
+        <f t="shared" si="0"/>
+        <v>539</v>
+      </c>
       <c r="G26" s="12"/>
       <c r="H26" s="12"/>
     </row>
@@ -4694,6 +5075,10 @@
       </c>
       <c r="E27" s="8">
         <v>12</v>
+      </c>
+      <c r="F27" s="16">
+        <f t="shared" si="0"/>
+        <v>2262</v>
       </c>
       <c r="G27" s="12"/>
       <c r="H27" s="12"/>

</xml_diff>

<commit_message>
Arreglando problema con los puntos
</commit_message>
<xml_diff>
--- a/Bases_de_Rama_Judicial-Cálculo_DEA.xlsx
+++ b/Bases_de_Rama_Judicial-Cálculo_DEA.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3000" windowWidth="24000" windowHeight="9216" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="4200" windowWidth="24000" windowHeight="9216"/>
   </bookViews>
   <sheets>
     <sheet name="circuito" sheetId="5" r:id="rId1"/>
@@ -495,7 +495,7 @@
     <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -530,13 +530,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Millares [0] 2" xfId="1"/>
@@ -821,8 +828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -855,19 +862,19 @@
       <c r="A2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="17">
         <v>360</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="17">
         <v>70</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="17">
         <v>716</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="17">
         <v>2</v>
       </c>
-      <c r="F2" s="16">
+      <c r="F2" s="18">
         <f>SUM(B2,D2)</f>
         <v>1076</v>
       </c>
@@ -876,19 +883,19 @@
       <c r="A3" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="17">
         <v>240</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="17">
         <v>81</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="17">
         <v>430</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="17">
         <v>6</v>
       </c>
-      <c r="F3" s="16">
+      <c r="F3" s="18">
         <f t="shared" ref="F3:F39" si="0">SUM(B3,D3)</f>
         <v>670</v>
       </c>
@@ -897,19 +904,19 @@
       <c r="A4" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="17">
         <v>68</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="17">
         <v>33</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="17">
         <v>102</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="17">
         <v>2</v>
       </c>
-      <c r="F4" s="16">
+      <c r="F4" s="18">
         <f t="shared" si="0"/>
         <v>170</v>
       </c>
@@ -918,19 +925,19 @@
       <c r="A5" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="17">
         <v>617</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="17">
         <v>270</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="17">
         <v>1218</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="17">
         <v>15</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F5" s="18">
         <f t="shared" si="0"/>
         <v>1835</v>
       </c>
@@ -939,19 +946,19 @@
       <c r="A6" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="17">
         <v>2926</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="17">
         <v>1468</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="17">
         <v>7632</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="17">
         <v>65</v>
       </c>
-      <c r="F6" s="16">
+      <c r="F6" s="18">
         <f t="shared" si="0"/>
         <v>10558</v>
       </c>
@@ -960,19 +967,19 @@
       <c r="A7" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="17">
         <v>434</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="17">
         <v>225</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="17">
         <v>553</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="17">
         <v>15</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F7" s="18">
         <f t="shared" si="0"/>
         <v>987</v>
       </c>
@@ -981,19 +988,19 @@
       <c r="A8" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="17">
         <v>107</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="17">
         <v>33</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="17">
         <v>221</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="17">
         <v>3</v>
       </c>
-      <c r="F8" s="16">
+      <c r="F8" s="18">
         <f t="shared" si="0"/>
         <v>328</v>
       </c>
@@ -1002,19 +1009,19 @@
       <c r="A9" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="17">
         <v>352</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="17">
         <v>122</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="17">
         <v>592</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="17">
         <v>3</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9" s="18">
         <f t="shared" si="0"/>
         <v>944</v>
       </c>
@@ -1023,19 +1030,19 @@
       <c r="A10" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="17">
         <v>978</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="17">
         <v>389</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="17">
         <v>2462</v>
       </c>
-      <c r="E10" s="8">
+      <c r="E10" s="17">
         <v>21</v>
       </c>
-      <c r="F10" s="16">
+      <c r="F10" s="18">
         <f t="shared" si="0"/>
         <v>3440</v>
       </c>
@@ -1044,19 +1051,19 @@
       <c r="A11" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="17">
         <v>554</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="17">
         <v>410</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="17">
         <v>1699</v>
       </c>
-      <c r="E11" s="8">
+      <c r="E11" s="17">
         <v>15</v>
       </c>
-      <c r="F11" s="16">
+      <c r="F11" s="18">
         <f t="shared" si="0"/>
         <v>2253</v>
       </c>
@@ -1065,19 +1072,19 @@
       <c r="A12" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="17">
         <v>317</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="17">
         <v>102</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="17">
         <v>1055</v>
       </c>
-      <c r="E12" s="8">
+      <c r="E12" s="17">
         <v>10</v>
       </c>
-      <c r="F12" s="16">
+      <c r="F12" s="18">
         <f t="shared" si="0"/>
         <v>1372</v>
       </c>
@@ -1086,19 +1093,19 @@
       <c r="A13" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="17">
         <v>47</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="17">
         <v>8</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="17">
         <v>82</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="17">
         <v>3</v>
       </c>
-      <c r="F13" s="16">
+      <c r="F13" s="18">
         <f t="shared" si="0"/>
         <v>129</v>
       </c>
@@ -1107,19 +1114,19 @@
       <c r="A14" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="17">
         <v>600</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="17">
         <v>187</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="17">
         <v>1151</v>
       </c>
-      <c r="E14" s="8">
+      <c r="E14" s="17">
         <v>4</v>
       </c>
-      <c r="F14" s="16">
+      <c r="F14" s="18">
         <f t="shared" si="0"/>
         <v>1751</v>
       </c>
@@ -1128,19 +1135,19 @@
       <c r="A15" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="17">
         <v>43</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="17">
         <v>11</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="17">
         <v>144</v>
       </c>
-      <c r="E15" s="8">
+      <c r="E15" s="17">
         <v>3</v>
       </c>
-      <c r="F15" s="16">
+      <c r="F15" s="18">
         <f t="shared" si="0"/>
         <v>187</v>
       </c>
@@ -1149,19 +1156,19 @@
       <c r="A16" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="17">
         <v>534</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="17">
         <v>173</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="17">
         <v>1251</v>
       </c>
-      <c r="E16" s="8">
+      <c r="E16" s="17">
         <v>12</v>
       </c>
-      <c r="F16" s="16">
+      <c r="F16" s="18">
         <f t="shared" si="0"/>
         <v>1785</v>
       </c>
@@ -1170,19 +1177,19 @@
       <c r="A17" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="17">
         <v>4</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="17">
         <v>4</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="17">
         <v>10</v>
       </c>
-      <c r="E17" s="8">
+      <c r="E17" s="17">
         <v>1</v>
       </c>
-      <c r="F17" s="16">
+      <c r="F17" s="18">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
@@ -1191,19 +1198,19 @@
       <c r="A18" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="17">
         <v>259</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="17">
         <v>55</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="17">
         <v>627</v>
       </c>
-      <c r="E18" s="8">
+      <c r="E18" s="17">
         <v>8</v>
       </c>
-      <c r="F18" s="16">
+      <c r="F18" s="18">
         <f t="shared" si="0"/>
         <v>886</v>
       </c>
@@ -1212,19 +1219,19 @@
       <c r="A19" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="17">
         <v>1247</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="17">
         <v>705</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="17">
         <v>3409</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19" s="17">
         <v>36</v>
       </c>
-      <c r="F19" s="16">
+      <c r="F19" s="18">
         <f t="shared" si="0"/>
         <v>4656</v>
       </c>
@@ -1233,19 +1240,19 @@
       <c r="A20" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="17">
         <v>493</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="17">
         <v>275</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="17">
         <v>407</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E20" s="17">
         <v>2</v>
       </c>
-      <c r="F20" s="16">
+      <c r="F20" s="18">
         <f t="shared" si="0"/>
         <v>900</v>
       </c>
@@ -1254,19 +1261,19 @@
       <c r="A21" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="17">
         <v>309</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="17">
         <v>121</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="17">
         <v>672</v>
       </c>
-      <c r="E21" s="8">
+      <c r="E21" s="17">
         <v>7</v>
       </c>
-      <c r="F21" s="16">
+      <c r="F21" s="18">
         <f t="shared" si="0"/>
         <v>981</v>
       </c>
@@ -1275,19 +1282,19 @@
       <c r="A22" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22" s="17">
         <v>406</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="17">
         <v>110</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="17">
         <v>1079</v>
       </c>
-      <c r="E22" s="8">
+      <c r="E22" s="17">
         <v>9</v>
       </c>
-      <c r="F22" s="16">
+      <c r="F22" s="18">
         <f t="shared" si="0"/>
         <v>1485</v>
       </c>
@@ -1296,19 +1303,19 @@
       <c r="A23" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23" s="17">
         <v>30</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="17">
         <v>24</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23" s="17">
         <v>75</v>
       </c>
-      <c r="E23" s="8">
+      <c r="E23" s="17">
         <v>1</v>
       </c>
-      <c r="F23" s="16">
+      <c r="F23" s="18">
         <f t="shared" si="0"/>
         <v>105</v>
       </c>
@@ -1317,19 +1324,19 @@
       <c r="A24" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24" s="17">
         <v>485</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="17">
         <v>776</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="17">
         <v>1056</v>
       </c>
-      <c r="E24" s="8">
+      <c r="E24" s="17">
         <v>9</v>
       </c>
-      <c r="F24" s="16">
+      <c r="F24" s="18">
         <f t="shared" si="0"/>
         <v>1541</v>
       </c>
@@ -1338,19 +1345,19 @@
       <c r="A25" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B25" s="17">
         <v>238</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C25" s="17">
         <v>114</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D25" s="17">
         <v>559</v>
       </c>
-      <c r="E25" s="8">
+      <c r="E25" s="17">
         <v>7</v>
       </c>
-      <c r="F25" s="16">
+      <c r="F25" s="18">
         <f t="shared" si="0"/>
         <v>797</v>
       </c>
@@ -1359,19 +1366,19 @@
       <c r="A26" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26" s="17">
         <v>790</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="17">
         <v>397</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D26" s="17">
         <v>2281</v>
       </c>
-      <c r="E26" s="8">
+      <c r="E26" s="17">
         <v>10</v>
       </c>
-      <c r="F26" s="16">
+      <c r="F26" s="18">
         <f t="shared" si="0"/>
         <v>3071</v>
       </c>
@@ -1380,19 +1387,19 @@
       <c r="A27" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B27" s="5">
+      <c r="B27" s="17">
         <v>371</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C27" s="17">
         <v>64</v>
       </c>
-      <c r="D27" s="5">
+      <c r="D27" s="17">
         <v>593</v>
       </c>
-      <c r="E27" s="8">
+      <c r="E27" s="17">
         <v>4</v>
       </c>
-      <c r="F27" s="16">
+      <c r="F27" s="18">
         <f t="shared" si="0"/>
         <v>964</v>
       </c>
@@ -1401,19 +1408,19 @@
       <c r="A28" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="5">
+      <c r="B28" s="17">
         <v>148</v>
       </c>
-      <c r="C28" s="5">
+      <c r="C28" s="17">
         <v>43</v>
       </c>
-      <c r="D28" s="5">
+      <c r="D28" s="17">
         <v>443</v>
       </c>
-      <c r="E28" s="8">
+      <c r="E28" s="17">
         <v>3</v>
       </c>
-      <c r="F28" s="16">
+      <c r="F28" s="18">
         <f t="shared" si="0"/>
         <v>591</v>
       </c>
@@ -1422,19 +1429,19 @@
       <c r="A29" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B29" s="5">
+      <c r="B29" s="17">
         <v>34</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C29" s="17">
         <v>13</v>
       </c>
-      <c r="D29" s="5">
+      <c r="D29" s="17">
         <v>101</v>
       </c>
-      <c r="E29" s="8">
+      <c r="E29" s="17">
         <v>1</v>
       </c>
-      <c r="F29" s="16">
+      <c r="F29" s="18">
         <f t="shared" si="0"/>
         <v>135</v>
       </c>
@@ -1443,19 +1450,19 @@
       <c r="A30" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="B30" s="5">
+      <c r="B30" s="17">
         <v>162</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C30" s="17">
         <v>51</v>
       </c>
-      <c r="D30" s="5">
+      <c r="D30" s="17">
         <v>139</v>
       </c>
-      <c r="E30" s="8">
+      <c r="E30" s="17">
         <v>3</v>
       </c>
-      <c r="F30" s="16">
+      <c r="F30" s="18">
         <f t="shared" si="0"/>
         <v>301</v>
       </c>
@@ -1464,19 +1471,19 @@
       <c r="A31" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B31" s="5">
+      <c r="B31" s="17">
         <v>323</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C31" s="17">
         <v>129</v>
       </c>
-      <c r="D31" s="5">
+      <c r="D31" s="17">
         <v>210</v>
       </c>
-      <c r="E31" s="4">
+      <c r="E31" s="19">
         <v>7</v>
       </c>
-      <c r="F31" s="16">
+      <c r="F31" s="18">
         <f t="shared" si="0"/>
         <v>533</v>
       </c>
@@ -1485,19 +1492,19 @@
       <c r="A32" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B32" s="5">
+      <c r="B32" s="17">
         <v>267</v>
       </c>
-      <c r="C32" s="5">
+      <c r="C32" s="17">
         <v>181</v>
       </c>
-      <c r="D32" s="5">
+      <c r="D32" s="17">
         <v>774</v>
       </c>
-      <c r="E32" s="8">
+      <c r="E32" s="17">
         <v>8</v>
       </c>
-      <c r="F32" s="16">
+      <c r="F32" s="18">
         <f t="shared" si="0"/>
         <v>1041</v>
       </c>
@@ -1506,19 +1513,19 @@
       <c r="A33" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="5">
+      <c r="B33" s="17">
         <v>243</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C33" s="17">
         <v>153</v>
       </c>
-      <c r="D33" s="5">
+      <c r="D33" s="17">
         <v>549</v>
       </c>
-      <c r="E33" s="8">
+      <c r="E33" s="17">
         <v>9</v>
       </c>
-      <c r="F33" s="16">
+      <c r="F33" s="18">
         <f t="shared" si="0"/>
         <v>792</v>
       </c>
@@ -1527,19 +1534,19 @@
       <c r="A34" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B34" s="5">
+      <c r="B34" s="17">
         <v>180</v>
       </c>
-      <c r="C34" s="5">
+      <c r="C34" s="17">
         <v>159</v>
       </c>
-      <c r="D34" s="5">
+      <c r="D34" s="17">
         <v>327</v>
       </c>
-      <c r="E34" s="8">
+      <c r="E34" s="17">
         <v>15</v>
       </c>
-      <c r="F34" s="16">
+      <c r="F34" s="18">
         <f t="shared" si="0"/>
         <v>507</v>
       </c>
@@ -1548,19 +1555,19 @@
       <c r="A35" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B35" s="5">
+      <c r="B35" s="17">
         <v>102</v>
       </c>
-      <c r="C35" s="5">
+      <c r="C35" s="17">
         <v>38</v>
       </c>
-      <c r="D35" s="5">
+      <c r="D35" s="17">
         <v>219</v>
       </c>
-      <c r="E35" s="8">
+      <c r="E35" s="17">
         <v>2</v>
       </c>
-      <c r="F35" s="16">
+      <c r="F35" s="18">
         <f t="shared" si="0"/>
         <v>321</v>
       </c>
@@ -1569,19 +1576,19 @@
       <c r="A36" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B36" s="5">
+      <c r="B36" s="17">
         <v>631</v>
       </c>
-      <c r="C36" s="5">
+      <c r="C36" s="17">
         <v>272</v>
       </c>
-      <c r="D36" s="5">
+      <c r="D36" s="17">
         <v>1235</v>
       </c>
-      <c r="E36" s="8">
+      <c r="E36" s="17">
         <v>8</v>
       </c>
-      <c r="F36" s="16">
+      <c r="F36" s="18">
         <f t="shared" si="0"/>
         <v>1866</v>
       </c>
@@ -1590,19 +1597,19 @@
       <c r="A37" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B37" s="5">
+      <c r="B37" s="17">
         <v>427</v>
       </c>
-      <c r="C37" s="5">
+      <c r="C37" s="17">
         <v>378</v>
       </c>
-      <c r="D37" s="5">
+      <c r="D37" s="17">
         <v>894</v>
       </c>
-      <c r="E37" s="8">
+      <c r="E37" s="17">
         <v>9</v>
       </c>
-      <c r="F37" s="16">
+      <c r="F37" s="18">
         <f t="shared" si="0"/>
         <v>1321</v>
       </c>
@@ -1611,19 +1618,19 @@
       <c r="A38" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="B38" s="5">
+      <c r="B38" s="17">
         <v>124</v>
       </c>
-      <c r="C38" s="5">
+      <c r="C38" s="17">
         <v>22</v>
       </c>
-      <c r="D38" s="5">
+      <c r="D38" s="17">
         <v>319</v>
       </c>
-      <c r="E38" s="8">
+      <c r="E38" s="17">
         <v>2</v>
       </c>
-      <c r="F38" s="16">
+      <c r="F38" s="18">
         <f t="shared" si="0"/>
         <v>443</v>
       </c>
@@ -1632,19 +1639,19 @@
       <c r="A39" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B39" s="5">
+      <c r="B39" s="17">
         <v>28</v>
       </c>
-      <c r="C39" s="5">
+      <c r="C39" s="17">
         <v>23</v>
       </c>
-      <c r="D39" s="5">
+      <c r="D39" s="17">
         <v>32</v>
       </c>
-      <c r="E39" s="8">
+      <c r="E39" s="17">
         <v>3</v>
       </c>
-      <c r="F39" s="16">
+      <c r="F39" s="18">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
@@ -1659,7 +1666,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -1673,56 +1680,56 @@
       <c r="A1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="16">
         <v>2016</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -1757,12 +1764,12 @@
       <c r="E8" s="1">
         <v>2</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="H8" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
@@ -1780,10 +1787,10 @@
       <c r="E9" s="1">
         <v>6</v>
       </c>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -1801,10 +1808,10 @@
       <c r="E10" s="1">
         <v>2</v>
       </c>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
-      <c r="K10" s="14"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
@@ -1822,10 +1829,10 @@
       <c r="E11" s="1">
         <v>15</v>
       </c>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
-      <c r="K11" s="14"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
@@ -2519,56 +2526,56 @@
       <c r="A1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="16">
         <v>2016</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -2641,11 +2648,11 @@
       <c r="E10" s="8">
         <v>15</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
@@ -2663,9 +2670,9 @@
       <c r="E11" s="8">
         <v>15</v>
       </c>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
@@ -2683,9 +2690,9 @@
       <c r="E12" s="8">
         <v>19</v>
       </c>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
@@ -2703,9 +2710,9 @@
       <c r="E13" s="8">
         <v>8</v>
       </c>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
@@ -3170,7 +3177,7 @@
       <c r="E2" s="7">
         <v>38</v>
       </c>
-      <c r="F2" s="16">
+      <c r="F2" s="14">
         <f>SUM(B2,D2)</f>
         <v>4977</v>
       </c>
@@ -3193,7 +3200,7 @@
       <c r="E3" s="7">
         <v>2</v>
       </c>
-      <c r="F3" s="16">
+      <c r="F3" s="14">
         <f t="shared" ref="F3:F27" si="0">SUM(B3,D3)</f>
         <v>1076</v>
       </c>
@@ -3216,7 +3223,7 @@
       <c r="E4" s="7">
         <v>15</v>
       </c>
-      <c r="F4" s="16">
+      <c r="F4" s="14">
         <f t="shared" si="0"/>
         <v>1835</v>
       </c>
@@ -3239,7 +3246,7 @@
       <c r="E5" s="7">
         <v>15</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F5" s="14">
         <f t="shared" si="0"/>
         <v>2253</v>
       </c>
@@ -3262,7 +3269,7 @@
       <c r="E6" s="7">
         <v>19</v>
       </c>
-      <c r="F6" s="16">
+      <c r="F6" s="14">
         <f t="shared" si="0"/>
         <v>1040</v>
       </c>
@@ -3285,7 +3292,7 @@
       <c r="E7" s="7">
         <v>8</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F7" s="14">
         <f t="shared" si="0"/>
         <v>886</v>
       </c>
@@ -3308,7 +3315,7 @@
       <c r="E8" s="7">
         <v>4</v>
       </c>
-      <c r="F8" s="16">
+      <c r="F8" s="14">
         <f t="shared" si="0"/>
         <v>1751</v>
       </c>
@@ -3331,7 +3338,7 @@
       <c r="E9" s="7">
         <v>2</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9" s="14">
         <f t="shared" si="0"/>
         <v>443</v>
       </c>
@@ -3354,7 +3361,7 @@
       <c r="E10" s="7">
         <v>10</v>
       </c>
-      <c r="F10" s="16">
+      <c r="F10" s="14">
         <f t="shared" si="0"/>
         <v>3071</v>
       </c>
@@ -3377,7 +3384,7 @@
       <c r="E11" s="7">
         <v>8</v>
       </c>
-      <c r="F11" s="16">
+      <c r="F11" s="14">
         <f t="shared" si="0"/>
         <v>1866</v>
       </c>
@@ -3400,7 +3407,7 @@
       <c r="E12" s="7">
         <v>4</v>
       </c>
-      <c r="F12" s="16">
+      <c r="F12" s="14">
         <f t="shared" si="0"/>
         <v>964</v>
       </c>
@@ -3423,7 +3430,7 @@
       <c r="E13" s="7">
         <v>7</v>
       </c>
-      <c r="F13" s="16">
+      <c r="F13" s="14">
         <f t="shared" si="0"/>
         <v>981</v>
       </c>
@@ -3446,7 +3453,7 @@
       <c r="E14" s="7">
         <v>75</v>
       </c>
-      <c r="F14" s="16">
+      <c r="F14" s="14">
         <f t="shared" si="0"/>
         <v>10948</v>
       </c>
@@ -3469,7 +3476,7 @@
       <c r="E15" s="7">
         <v>3</v>
       </c>
-      <c r="F15" s="16">
+      <c r="F15" s="14">
         <f t="shared" si="0"/>
         <v>591</v>
       </c>
@@ -3492,7 +3499,7 @@
       <c r="E16" s="7">
         <v>9</v>
       </c>
-      <c r="F16" s="16">
+      <c r="F16" s="14">
         <f t="shared" si="0"/>
         <v>1485</v>
       </c>
@@ -3515,7 +3522,7 @@
       <c r="E17" s="7">
         <v>8</v>
       </c>
-      <c r="F17" s="16">
+      <c r="F17" s="14">
         <f t="shared" si="0"/>
         <v>1041</v>
       </c>
@@ -3538,7 +3545,7 @@
       <c r="E18" s="7">
         <v>9</v>
       </c>
-      <c r="F18" s="16">
+      <c r="F18" s="14">
         <f t="shared" si="0"/>
         <v>1321</v>
       </c>
@@ -3561,7 +3568,7 @@
       <c r="E19" s="7">
         <v>11</v>
       </c>
-      <c r="F19" s="16">
+      <c r="F19" s="14">
         <f t="shared" si="0"/>
         <v>2441</v>
       </c>
@@ -3584,7 +3591,7 @@
       <c r="E20" s="7">
         <v>11</v>
       </c>
-      <c r="F20" s="16">
+      <c r="F20" s="14">
         <f t="shared" si="0"/>
         <v>1477</v>
       </c>
@@ -3607,7 +3614,7 @@
       <c r="E21" s="7">
         <v>6</v>
       </c>
-      <c r="F21" s="16">
+      <c r="F21" s="14">
         <f t="shared" si="0"/>
         <v>670</v>
       </c>
@@ -3630,7 +3637,7 @@
       <c r="E22" s="7">
         <v>7</v>
       </c>
-      <c r="F22" s="16">
+      <c r="F22" s="14">
         <f t="shared" si="0"/>
         <v>797</v>
       </c>
@@ -3653,7 +3660,7 @@
       <c r="E23" s="7">
         <v>1</v>
       </c>
-      <c r="F23" s="16">
+      <c r="F23" s="14">
         <f t="shared" si="0"/>
         <v>135</v>
       </c>
@@ -3676,7 +3683,7 @@
       <c r="E24" s="7">
         <v>20</v>
       </c>
-      <c r="F24" s="16">
+      <c r="F24" s="14">
         <f t="shared" si="0"/>
         <v>1458</v>
       </c>
@@ -3699,7 +3706,7 @@
       <c r="E25" s="7">
         <v>9</v>
       </c>
-      <c r="F25" s="16">
+      <c r="F25" s="14">
         <f t="shared" si="0"/>
         <v>792</v>
       </c>
@@ -3722,7 +3729,7 @@
       <c r="E26" s="7">
         <v>12</v>
       </c>
-      <c r="F26" s="16">
+      <c r="F26" s="14">
         <f t="shared" si="0"/>
         <v>1785</v>
       </c>
@@ -3745,7 +3752,7 @@
       <c r="E27" s="7">
         <v>29</v>
       </c>
-      <c r="F27" s="16">
+      <c r="F27" s="14">
         <f t="shared" si="0"/>
         <v>4712</v>
       </c>
@@ -3772,56 +3779,56 @@
       <c r="A1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="16">
         <v>2016</v>
       </c>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -4501,7 +4508,7 @@
       <c r="E2" s="8">
         <v>15</v>
       </c>
-      <c r="F2" s="16">
+      <c r="F2" s="14">
         <f>SUM(B2,D2)</f>
         <v>2465</v>
       </c>
@@ -4524,7 +4531,7 @@
       <c r="E3" s="8">
         <v>3</v>
       </c>
-      <c r="F3" s="16">
+      <c r="F3" s="14">
         <f t="shared" ref="F3:F27" si="0">SUM(B3,D3)</f>
         <v>212</v>
       </c>
@@ -4547,7 +4554,7 @@
       <c r="E4" s="8">
         <v>9</v>
       </c>
-      <c r="F4" s="16">
+      <c r="F4" s="14">
         <f t="shared" si="0"/>
         <v>793</v>
       </c>
@@ -4570,7 +4577,7 @@
       <c r="E5" s="8">
         <v>6</v>
       </c>
-      <c r="F5" s="16">
+      <c r="F5" s="14">
         <f t="shared" si="0"/>
         <v>1019</v>
       </c>
@@ -4593,7 +4600,7 @@
       <c r="E6" s="8">
         <v>6</v>
       </c>
-      <c r="F6" s="16">
+      <c r="F6" s="14">
         <f t="shared" si="0"/>
         <v>653</v>
       </c>
@@ -4616,7 +4623,7 @@
       <c r="E7" s="8">
         <v>6</v>
       </c>
-      <c r="F7" s="16">
+      <c r="F7" s="14">
         <f t="shared" si="0"/>
         <v>415</v>
       </c>
@@ -4639,7 +4646,7 @@
       <c r="E8" s="8">
         <v>4</v>
       </c>
-      <c r="F8" s="16">
+      <c r="F8" s="14">
         <f t="shared" si="0"/>
         <v>1012</v>
       </c>
@@ -4662,7 +4669,7 @@
       <c r="E9" s="8">
         <v>3</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9" s="14">
         <f t="shared" si="0"/>
         <v>224</v>
       </c>
@@ -4685,7 +4692,7 @@
       <c r="E10" s="8">
         <v>5</v>
       </c>
-      <c r="F10" s="16">
+      <c r="F10" s="14">
         <f t="shared" si="0"/>
         <v>1071</v>
       </c>
@@ -4708,7 +4715,7 @@
       <c r="E11" s="8">
         <v>4</v>
       </c>
-      <c r="F11" s="16">
+      <c r="F11" s="14">
         <f t="shared" si="0"/>
         <v>638</v>
       </c>
@@ -4731,7 +4738,7 @@
       <c r="E12" s="8">
         <v>3</v>
       </c>
-      <c r="F12" s="16">
+      <c r="F12" s="14">
         <f t="shared" si="0"/>
         <v>348</v>
       </c>
@@ -4754,7 +4761,7 @@
       <c r="E13" s="8">
         <v>4</v>
       </c>
-      <c r="F13" s="16">
+      <c r="F13" s="14">
         <f t="shared" si="0"/>
         <v>471</v>
       </c>
@@ -4777,7 +4784,7 @@
       <c r="E14" s="8">
         <v>9</v>
       </c>
-      <c r="F14" s="16">
+      <c r="F14" s="14">
         <f t="shared" si="0"/>
         <v>3729</v>
       </c>
@@ -4800,7 +4807,7 @@
       <c r="E15" s="8">
         <v>3</v>
       </c>
-      <c r="F15" s="16">
+      <c r="F15" s="14">
         <f t="shared" si="0"/>
         <v>180</v>
       </c>
@@ -4823,7 +4830,7 @@
       <c r="E16" s="8">
         <v>6</v>
       </c>
-      <c r="F16" s="16">
+      <c r="F16" s="14">
         <f t="shared" si="0"/>
         <v>486</v>
       </c>
@@ -4846,7 +4853,7 @@
       <c r="E17" s="8">
         <v>4</v>
       </c>
-      <c r="F17" s="16">
+      <c r="F17" s="14">
         <f t="shared" si="0"/>
         <v>506</v>
       </c>
@@ -4869,7 +4876,7 @@
       <c r="E18" s="8">
         <v>5</v>
       </c>
-      <c r="F18" s="16">
+      <c r="F18" s="14">
         <f t="shared" si="0"/>
         <v>1539</v>
       </c>
@@ -4892,7 +4899,7 @@
       <c r="E19" s="8">
         <v>6</v>
       </c>
-      <c r="F19" s="16">
+      <c r="F19" s="14">
         <f t="shared" si="0"/>
         <v>1263</v>
       </c>
@@ -4915,7 +4922,7 @@
       <c r="E20" s="8">
         <v>5</v>
       </c>
-      <c r="F20" s="16">
+      <c r="F20" s="14">
         <f t="shared" si="0"/>
         <v>675</v>
       </c>
@@ -4938,7 +4945,7 @@
       <c r="E21" s="8">
         <v>5</v>
       </c>
-      <c r="F21" s="16">
+      <c r="F21" s="14">
         <f t="shared" si="0"/>
         <v>521</v>
       </c>
@@ -4961,7 +4968,7 @@
       <c r="E22" s="8">
         <v>4</v>
       </c>
-      <c r="F22" s="16">
+      <c r="F22" s="14">
         <f t="shared" si="0"/>
         <v>559</v>
       </c>
@@ -4984,7 +4991,7 @@
       <c r="E23" s="8">
         <v>3</v>
       </c>
-      <c r="F23" s="16">
+      <c r="F23" s="14">
         <f t="shared" si="0"/>
         <v>101</v>
       </c>
@@ -5007,7 +5014,7 @@
       <c r="E24" s="8">
         <v>6</v>
       </c>
-      <c r="F24" s="16">
+      <c r="F24" s="14">
         <f t="shared" si="0"/>
         <v>974</v>
       </c>
@@ -5030,7 +5037,7 @@
       <c r="E25" s="8">
         <v>4</v>
       </c>
-      <c r="F25" s="16">
+      <c r="F25" s="14">
         <f t="shared" si="0"/>
         <v>438</v>
       </c>
@@ -5053,7 +5060,7 @@
       <c r="E26" s="8">
         <v>6</v>
       </c>
-      <c r="F26" s="16">
+      <c r="F26" s="14">
         <f t="shared" si="0"/>
         <v>539</v>
       </c>
@@ -5076,7 +5083,7 @@
       <c r="E27" s="8">
         <v>12</v>
       </c>
-      <c r="F27" s="16">
+      <c r="F27" s="14">
         <f t="shared" si="0"/>
         <v>2262</v>
       </c>

</xml_diff>